<commit_message>
Update IP - EX 16 - Trabalhando com a matematica (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 16 - Trabalhando com a matematica (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 16 - Trabalhando com a matematica (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E1FD6B3-8C6A-4E4F-B1E3-85A0160637A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC769DF-BFEA-4C98-B49B-42617D8D46B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,6 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1288,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:R20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1298,7 @@
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="1.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="0.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1421,13 +1422,18 @@
         <v>13</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="17"/>
+      <c r="E10" s="17">
+        <f>I12*I10*I14</f>
+        <v>750000</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="19" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="17"/>
+      <c r="I10" s="17">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="2:18" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21"/>
@@ -1435,6 +1441,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="19"/>
       <c r="H11" s="3"/>
+      <c r="I11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
@@ -1444,13 +1453,18 @@
         <v>14</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="17"/>
+      <c r="E12" s="40">
+        <f>(I14/I10)/I12</f>
+        <v>0.03</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="17"/>
+      <c r="I12" s="17">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="2:18" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="21"/>
@@ -1467,13 +1481,18 @@
         <v>15</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="17">
+        <f>I10+I12+I14</f>
+        <v>300</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="19" t="s">
         <v>4</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="17"/>
+      <c r="I14" s="17">
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="2:18" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="21"/>
@@ -1487,7 +1506,10 @@
         <v>10</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="17"/>
+      <c r="E16" s="17">
+        <f>SQRT(I12)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="2:5" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="21"/>
@@ -1501,7 +1523,10 @@
         <v>16</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="17"/>
+      <c r="E18" s="17">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
     </row>
     <row r="19" spans="2:5" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="21"/>
@@ -1515,7 +1540,10 @@
         <v>17</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="17">
+        <f>I10^I12</f>
+        <v>7.8886090522101218E+169</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>